<commit_message>
Preschool: prep desample for school, integration of alt forms
</commit_message>
<xml_diff>
--- a/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
+++ b/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/SPM2-R/INPUT-FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB66096-29C6-DC47-8D81-C374E79A60F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DB5186-1548-4B40-A583-F6E9603B59E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{050599CA-26A7-BA4B-BEE7-0D734EED4004}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{050599CA-26A7-BA4B-BEE7-0D734EED4004}"/>
   </bookViews>
   <sheets>
     <sheet name="normDataSource" sheetId="2" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -667,20 +667,20 @@
         <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -692,13 +692,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -832,20 +832,20 @@
         <v>13</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I11" s="12"/>
     </row>
@@ -857,13 +857,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -876,20 +876,20 @@
         <v>7</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I13" s="12"/>
     </row>

</xml_diff>

<commit_message>
verifying inputs to IT norms desample
</commit_message>
<xml_diff>
--- a/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
+++ b/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/SPM2-R/INPUT-FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DB5186-1548-4B40-A583-F6E9603B59E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D562E3E-6B9F-9C49-A60E-393892BBA374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{050599CA-26A7-BA4B-BEE7-0D734EED4004}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -786,23 +786,23 @@
         <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -813,13 +813,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>

</xml_diff>

<commit_message>
IT norms output complete
</commit_message>
<xml_diff>
--- a/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
+++ b/INPUT-FILES/SPM-2-normDataSource-byForm.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/SPM2-R/INPUT-FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D562E3E-6B9F-9C49-A60E-393892BBA374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33977F6-8E0A-2440-8ABC-1A327CC8A0D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{050599CA-26A7-BA4B-BEE7-0D734EED4004}"/>
   </bookViews>
   <sheets>
     <sheet name="normDataSource" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,9 +101,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>XX = integrated into norms-output</t>
-  </si>
-  <si>
     <t>XX</t>
   </si>
   <si>
@@ -126,12 +123,15 @@
       <t xml:space="preserve"> = data exists but will not be used</t>
     </r>
   </si>
+  <si>
+    <t>XX = integrated into norms output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +151,13 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -224,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -255,6 +262,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +587,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -619,20 +632,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="8"/>
     </row>
@@ -644,7 +657,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="15" t="s">
@@ -652,10 +665,10 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="8"/>
     </row>
@@ -667,20 +680,20 @@
         <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -692,13 +705,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -711,22 +724,22 @@
         <v>15</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I6" s="10"/>
     </row>
@@ -738,22 +751,22 @@
         <v>16</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I7" s="10"/>
     </row>
@@ -786,23 +799,23 @@
         <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -813,13 +826,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -832,20 +845,20 @@
         <v>13</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="12"/>
     </row>
@@ -857,13 +870,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -876,31 +889,31 @@
         <v>7</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="12"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>